<commit_message>
updated the sorting functionality.
</commit_message>
<xml_diff>
--- a/PlanYourDegree.Docs/PorjectCostEstimate.xlsx
+++ b/PlanYourDegree.Docs/PorjectCostEstimate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Total value earned this point</t>
+  </si>
+  <si>
+    <t>Takehome Amout for developer</t>
   </si>
 </sst>
 </file>
@@ -402,22 +405,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -433,7 +435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -441,7 +443,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -454,8 +456,11 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -469,8 +474,12 @@
         <f>$B$3*C6</f>
         <v>1600</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <f>B6*$B$3</f>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -484,8 +493,12 @@
         <f t="shared" ref="D7:D10" si="0">$B$3*C7</f>
         <v>1600</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <f t="shared" ref="E7:E10" si="1">B7*$B$3</f>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -499,8 +512,12 @@
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -514,8 +531,12 @@
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -529,8 +550,12 @@
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -543,7 +568,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -551,7 +576,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -560,7 +585,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -568,7 +593,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>